<commit_message>
handling empty cells with validations
</commit_message>
<xml_diff>
--- a/CHLE2E/Data/LoginData.xlsx
+++ b/CHLE2E/Data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\CHLE2E\CHLE2E\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6077976C-2AC6-49B1-9065-6C89EDC5EA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD7829-BBFA-459C-BFF2-9D3B732E1F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>20-12-2022</t>
+  </si>
+  <si>
+    <t>Bhaldar</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,6 +509,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Patient List - created patient check
</commit_message>
<xml_diff>
--- a/CHLE2E/Data/LoginData.xlsx
+++ b/CHLE2E/Data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\CHLE2E\CHLE2E\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD7829-BBFA-459C-BFF2-9D3B732E1F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE83086-6ED0-4B14-9325-E7528AE4BEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -73,13 +73,22 @@
     <t>Chennai</t>
   </si>
   <si>
-    <t>febpatienttest@gmail.com</t>
-  </si>
-  <si>
     <t>20-12-2022</t>
   </si>
   <si>
-    <t>Bhaldar</t>
+    <t>+917676567656</t>
+  </si>
+  <si>
+    <t>Test Agency 1.1 (performance testing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency Test Patient(feb) </t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>febpatienttestt@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -463,13 +472,13 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7265625" customWidth="1"/>
     <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" customWidth="1"/>
@@ -509,18 +518,26 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="G2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Creating sensors through excel data
</commit_message>
<xml_diff>
--- a/CHLE2E/Data/LoginData.xlsx
+++ b/CHLE2E/Data/LoginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\CHLE2E\CHLE2E\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE83086-6ED0-4B14-9325-E7528AE4BEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D83517F-D7BA-46F0-9CFE-B7B76A2229CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>Test@123</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Chennai</t>
   </si>
   <si>
@@ -82,13 +79,16 @@
     <t>Test Agency 1.1 (performance testing)</t>
   </si>
   <si>
-    <t xml:space="preserve">Agency Test Patient(feb) </t>
-  </si>
-  <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>febpatienttestt@gmail.com</t>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>hanzo</t>
+  </si>
+  <si>
+    <t>Miya</t>
+  </si>
+  <si>
+    <t>miyaaa@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,13 +519,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>20</v>
@@ -534,16 +534,16 @@
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>